<commit_message>
Added grip test videos and more scripts for graphs
</commit_message>
<xml_diff>
--- a/Final Report/Experimental Data/Dynamometer vs Pressure.xlsx
+++ b/Final Report/Experimental Data/Dynamometer vs Pressure.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew\Documents\GitHub\Hydraulic-Mimic-Arm\Final Report\Experimental Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arobo\Documents\GitHub\Hydraulic-Mimic-Arm\Final Report\Experimental Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75002E8B-CDC8-4670-B2C0-6FC47CE1F71B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF87E5D-59F0-4FF2-AE81-673948DC7F79}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7965" activeTab="2" xr2:uid="{83A5CEDF-E666-4F4A-BF91-CC0FB8030E4B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7965" xr2:uid="{83A5CEDF-E666-4F4A-BF91-CC0FB8030E4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Dynanometer vs Pressure" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="36">
   <si>
     <t>pressure</t>
   </si>
@@ -77,6 +77,69 @@
   </si>
   <si>
     <t>Dynamometer (kg)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">600000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87.162226N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">800000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 116.216302N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1000000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 145.270377N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1200000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 174.324453N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1400000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 203.378528N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1600000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 232.432604N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1800000Pa </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 261.486679N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 65.956276N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 87.302348N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 108.648420N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 129.994492N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 151.340563N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 172.686635N</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 194.032707N</t>
   </si>
 </sst>
 </file>
@@ -332,6 +395,196 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-72CD-4489-835E-5AE70E81E2D1}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Theoretical</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dynanometer vs Pressure'!$F$23:$F$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dynanometer vs Pressure'!$G$23:$G$29</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>8.8850377166156989</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11.846717635066259</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.808396534148828</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17.77007645259939</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.731755351681958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>23.693435270132518</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.655114169215086</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-6939-4FF2-965F-EB5ED90821C6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Theoretical with Experimental Force</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Dynanometer vs Pressure'!$F$31:$F$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Dynanometer vs Pressure'!$G$31:$G$37</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>6.7233710499490318</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.8993211009174313</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>11.075272171253822</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>13.251222222222223</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15.427172273190623</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>17.60312232415902</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>19.77907237512742</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A934-40E0-8727-273B9564EC3E}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -593,6 +846,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3659,16 +3943,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>371475</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>147637</xdr:rowOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4075,10 +4359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8929C082-F7D1-4295-862C-786A2D8F6EE2}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4204,6 +4488,268 @@
       <c r="D8">
         <f>A8/10</f>
         <v>0.18</v>
+      </c>
+    </row>
+    <row r="23" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>16</v>
+      </c>
+      <c r="F23">
+        <f>_xlfn.NUMBERVALUE(LEFT(D23,LEN(D23)-3))/1000000</f>
+        <v>0.6</v>
+      </c>
+      <c r="G23">
+        <f>_xlfn.NUMBERVALUE(MID(E23,2,LEN(E23)-3))/9.81</f>
+        <v>8.8850377166156989</v>
+      </c>
+    </row>
+    <row r="24" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24">
+        <f t="shared" ref="F24:F30" si="2">_xlfn.NUMBERVALUE(LEFT(D24,LEN(D24)-3))/1000000</f>
+        <v>0.8</v>
+      </c>
+      <c r="G24">
+        <f t="shared" ref="G24:G30" si="3">_xlfn.NUMBERVALUE(MID(E24,2,LEN(E24)-3))/9.81</f>
+        <v>11.846717635066259</v>
+      </c>
+    </row>
+    <row r="25" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="3"/>
+        <v>14.808396534148828</v>
+      </c>
+    </row>
+    <row r="26" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>22</v>
+      </c>
+      <c r="F26">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="3"/>
+        <v>17.77007645259939</v>
+      </c>
+    </row>
+    <row r="27" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D27" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" t="s">
+        <v>24</v>
+      </c>
+      <c r="F27">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="3"/>
+        <v>20.731755351681958</v>
+      </c>
+    </row>
+    <row r="28" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="3"/>
+        <v>23.693435270132518</v>
+      </c>
+    </row>
+    <row r="29" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>27</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29">
+        <f t="shared" si="2"/>
+        <v>1.8</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="3"/>
+        <v>26.655114169215086</v>
+      </c>
+    </row>
+    <row r="30" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="F30" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G30" t="e">
+        <f t="shared" si="3"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="31" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" t="s">
+        <v>29</v>
+      </c>
+      <c r="F31">
+        <f t="shared" ref="F31:F37" si="4">_xlfn.NUMBERVALUE(LEFT(D31,LEN(D31)-3))/1000000</f>
+        <v>0.6</v>
+      </c>
+      <c r="G31">
+        <f t="shared" ref="G31:G37" si="5">_xlfn.NUMBERVALUE(MID(E31,2,LEN(E31)-3))/9.81</f>
+        <v>6.7233710499490318</v>
+      </c>
+      <c r="J31">
+        <f>G31/B2</f>
+        <v>1.6808427624872579</v>
+      </c>
+    </row>
+    <row r="32" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="E32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F32">
+        <f t="shared" si="4"/>
+        <v>0.8</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>8.8993211009174313</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32:J37" si="6">G32/B3</f>
+        <v>1.6180583819849874</v>
+      </c>
+    </row>
+    <row r="33" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>11.075272171253822</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="6"/>
+        <v>1.8771647747887832</v>
+      </c>
+    </row>
+    <row r="34" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D34" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="F34">
+        <f t="shared" si="4"/>
+        <v>1.2</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>13.251222222222223</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="6"/>
+        <v>1.8930317460317461</v>
+      </c>
+    </row>
+    <row r="35" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D35" t="s">
+        <v>23</v>
+      </c>
+      <c r="E35" t="s">
+        <v>33</v>
+      </c>
+      <c r="F35">
+        <f t="shared" si="4"/>
+        <v>1.4</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="5"/>
+        <v>15.427172273190623</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="6"/>
+        <v>1.9283965341488278</v>
+      </c>
+    </row>
+    <row r="36" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D36" t="s">
+        <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36">
+        <f t="shared" si="4"/>
+        <v>1.6</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="5"/>
+        <v>17.60312232415902</v>
+      </c>
+      <c r="J36">
+        <f t="shared" si="6"/>
+        <v>1.8054484435034892</v>
+      </c>
+    </row>
+    <row r="37" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D37" t="s">
+        <v>27</v>
+      </c>
+      <c r="E37" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37">
+        <f t="shared" si="4"/>
+        <v>1.8</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="5"/>
+        <v>19.77907237512742</v>
+      </c>
+      <c r="J37">
+        <f t="shared" si="6"/>
+        <v>1.8837211785835639</v>
       </c>
     </row>
   </sheetData>
@@ -4456,7 +5002,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8053FA6-F505-435E-9AC5-03C18D67843A}">
   <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>

</xml_diff>